<commit_message>
Add change password, editing users
</commit_message>
<xml_diff>
--- a/MyWebApplication/slon.xlsx
+++ b/MyWebApplication/slon.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Jkhfhg" sheetId="1" r:id="rId1"/>
-    <sheet name="Salo" sheetId="2" r:id="rId2"/>
-    <sheet name="Fender" sheetId="3" r:id="rId3"/>
+    <sheet name="Fender" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,10 +28,10 @@
     <t>Acoustic</t>
   </si>
   <si>
-    <t>Saf</t>
+    <t>Paint</t>
   </si>
   <si>
-    <t>Maplehgjhf</t>
+    <t>Good</t>
   </si>
 </sst>
 </file>
@@ -352,9 +351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -364,7 +361,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>34</v>
@@ -376,7 +373,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -388,20 +385,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Users page, Report.docx,
</commit_message>
<xml_diff>
--- a/MyWebApplication/slon.xlsx
+++ b/MyWebApplication/slon.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Jkhfhg" sheetId="1" r:id="rId1"/>
+    <sheet name="Squier" sheetId="1" r:id="rId1"/>
     <sheet name="Fender" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Stratocaster</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>Exlda</t>
+  </si>
+  <si>
+    <t>Olha</t>
+  </si>
+  <si>
+    <t>Superstrat</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -386,14 +397,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>1000</v>
+      </c>
+      <c r="C1">
+        <v>2001</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>